<commit_message>
prevented function from running if excel is closed
</commit_message>
<xml_diff>
--- a/GHEtool/GHETool.xlsx
+++ b/GHEtool/GHETool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BARC\repos\GHEtool2\GHEtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C0B01F-F02E-48AD-9F4A-3D66EC4E76B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA2CEA2-819A-4E1E-A9B6-B1E38229839C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{BFF6B84B-9156-4E9C-8343-263B9C198A37}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{BFF6B84B-9156-4E9C-8343-263B9C198A37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,9 @@
     <definedName name="bh_spacing">Sheet1!$D$5</definedName>
     <definedName name="bh_width">Sheet1!$D$6</definedName>
     <definedName name="cooling_demand">Sheet1!$G$4</definedName>
-    <definedName name="cooling_peak">Sheet1!$J$4</definedName>
+    <definedName name="cooling_peak">Sheet1!$L$4</definedName>
     <definedName name="heating_demand">Sheet1!$F$4</definedName>
-    <definedName name="heating_peak">Sheet1!$I$4</definedName>
+    <definedName name="heating_peak">Sheet1!$K$4</definedName>
     <definedName name="results_depth">Sheet1!$D$14</definedName>
     <definedName name="soil_conductivity">Sheet1!$D$10</definedName>
     <definedName name="soil_temperature">Sheet1!$D$11</definedName>
@@ -126,10 +126,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0\ &quot;W/m²&quot;"/>
-    <numFmt numFmtId="169" formatCode="0.0\ &quot;kWh/m²&quot;"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0\ &quot;W/m²&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.0\ &quot;kWh/m²&quot;"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -242,13 +243,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -258,8 +256,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -272,8 +270,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,40 +591,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4A2CE6-E4D6-4457-8D18-1B1AF7C129BB}">
-  <dimension ref="B2:J18"/>
+  <dimension ref="B2:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>1951</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3"/>
       <c r="C3"/>
       <c r="F3" s="2" t="s">
@@ -631,321 +633,425 @@
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>110</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>6</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>14360</v>
       </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="17">
+        <f>+F5/$F$17</f>
+        <v>0.20207421583665197</v>
+      </c>
+      <c r="I5" s="17">
+        <f>+G5/$G$17</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
         <v>53.333333333333336</v>
       </c>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="11" t="s">
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>5</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>11569</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>19</v>
       </c>
-      <c r="I6" s="5">
+      <c r="H6" s="17">
+        <f t="shared" ref="H6:H16" si="0">+F6/$F$17</f>
+        <v>0.16279920633803807</v>
+      </c>
+      <c r="I6" s="17">
+        <f t="shared" ref="I6:I16" si="1">+G6/$G$17</f>
+        <v>1.1796845895939401E-3</v>
+      </c>
+      <c r="K6" s="4">
         <v>47.333333333333336</v>
       </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="11" t="s">
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>4</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>8547</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>35</v>
       </c>
-      <c r="I7" s="5">
+      <c r="H7" s="17">
+        <f t="shared" si="0"/>
+        <v>0.12027356008049196</v>
+      </c>
+      <c r="I7" s="17">
+        <f t="shared" si="1"/>
+        <v>2.1731031913572582E-3</v>
+      </c>
+      <c r="K7" s="4">
         <v>34</v>
       </c>
-      <c r="J7" s="5">
+      <c r="L7" s="4">
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>0.15</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>5137</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>239</v>
       </c>
-      <c r="I8" s="5">
+      <c r="H8" s="17">
+        <f t="shared" si="0"/>
+        <v>7.2287969829587836E-2</v>
+      </c>
+      <c r="I8" s="17">
+        <f t="shared" si="1"/>
+        <v>1.4839190363839563E-2</v>
+      </c>
+      <c r="K8" s="4">
         <v>18.333333333333332</v>
       </c>
-      <c r="J8" s="5">
+      <c r="L8" s="4">
         <v>17.25</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="F9" s="5">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="F9" s="4">
         <v>1360</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>1346</v>
       </c>
-      <c r="I9" s="5">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
+      <c r="H9" s="17">
+        <f t="shared" si="0"/>
+        <v>1.9137948017955899E-2</v>
+      </c>
+      <c r="I9" s="17">
+        <f t="shared" si="1"/>
+        <v>8.3571339873339132E-2</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
         <v>33.25</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>3.5</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>368</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>2110</v>
       </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5">
+      <c r="H10" s="17">
+        <f t="shared" si="0"/>
+        <v>5.1785035813292427E-3</v>
+      </c>
+      <c r="I10" s="17">
+        <f t="shared" si="1"/>
+        <v>0.13100707810753756</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
         <v>46.75</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="11" t="s">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>10</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>208</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>5741</v>
       </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
+      <c r="H11" s="17">
+        <f t="shared" si="0"/>
+        <v>2.9269802850991375E-3</v>
+      </c>
+      <c r="I11" s="17">
+        <f t="shared" si="1"/>
+        <v>0.35645101204520052</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
         <v>53.25</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="F12" s="5">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="F12" s="4">
         <v>293</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>5105</v>
       </c>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
+      <c r="H12" s="17">
+        <f t="shared" si="0"/>
+        <v>4.1231020362213809E-3</v>
+      </c>
+      <c r="I12" s="17">
+        <f t="shared" si="1"/>
+        <v>0.31696262262510866</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="14" t="s">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>1207</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>1178</v>
       </c>
-      <c r="I13" s="5">
+      <c r="H13" s="17">
+        <f t="shared" si="0"/>
+        <v>1.6984928865935861E-2</v>
+      </c>
+      <c r="I13" s="17">
+        <f t="shared" si="1"/>
+        <v>7.3140444554824283E-2</v>
+      </c>
+      <c r="K13" s="4">
         <v>13.333333333333334</v>
       </c>
-      <c r="J13" s="5">
+      <c r="L13" s="4">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>103.53285093712304</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>4013</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>325</v>
       </c>
-      <c r="I14" s="5">
+      <c r="H14" s="17">
+        <f t="shared" si="0"/>
+        <v>5.6471018673571335E-2</v>
+      </c>
+      <c r="I14" s="17">
+        <f t="shared" si="1"/>
+        <v>2.0178815348317398E-2</v>
+      </c>
+      <c r="K14" s="4">
         <v>28.333333333333332</v>
       </c>
-      <c r="J14" s="5">
+      <c r="L14" s="4">
         <v>9.25</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="11" t="s">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="15">
         <f>+results_depth/bh_depth</f>
         <v>0.94120773579202766</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>10056</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>8</v>
       </c>
-      <c r="I15" s="5">
+      <c r="H15" s="17">
+        <f t="shared" si="0"/>
+        <v>0.14150823916806216</v>
+      </c>
+      <c r="I15" s="17">
+        <f t="shared" si="1"/>
+        <v>4.9670930088165902E-4</v>
+      </c>
+      <c r="K15" s="4">
         <v>39.666666666666664</v>
       </c>
-      <c r="J15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="14"/>
-      <c r="F16" s="5">
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B16" s="13"/>
+      <c r="F16" s="4">
         <v>13945</v>
       </c>
-      <c r="G16" s="5">
-        <v>0</v>
-      </c>
-      <c r="I16" s="5">
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="17">
+        <f t="shared" si="0"/>
+        <v>0.19623432728705514</v>
+      </c>
+      <c r="I16" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
         <v>45.333333333333336</v>
       </c>
-      <c r="J16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F17" s="6">
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F17" s="5">
         <f>+SUM(F5:F16)</f>
         <v>71063</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <f>+SUM(G5:G16)</f>
         <v>16106</v>
       </c>
-      <c r="I17" s="6">
-        <f>+MAX(I5:I16)</f>
+      <c r="H17" s="5">
+        <f t="shared" ref="H17:I17" si="2">+SUM(H5:H16)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K17" s="5">
+        <f>+MAX(K5:K16)</f>
         <v>53.333333333333336</v>
       </c>
-      <c r="J17" s="6">
-        <f>+MAX(J5:J16)</f>
+      <c r="L17" s="5">
+        <f>+MAX(L5:L16)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.35">
-      <c r="F18" s="8">
+    <row r="18" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F18" s="7">
         <f>+F17/$D$2</f>
         <v>36.423885187083549</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <f>+G17/$D$2</f>
         <v>8.2552537160430557</v>
       </c>
-      <c r="I18" s="7">
-        <f>+I17/$D$2*1000</f>
+      <c r="K18" s="6">
+        <f>+K17/$D$2*1000</f>
         <v>27.336408679309756</v>
       </c>
-      <c r="J18" s="7">
-        <f>+J17/$D$2*1000</f>
+      <c r="L18" s="6">
+        <f>+L17/$D$2*1000</f>
         <v>30.753459764223475</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>